<commit_message>
Update data for RASIO KBMI 4
</commit_message>
<xml_diff>
--- a/data/Rasio-KBMI-4.xlsx
+++ b/data/Rasio-KBMI-4.xlsx
@@ -4267,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>0</v>
+        <v>0.0469</v>
       </c>
       <c r="Q46" t="n">
         <v>0.005</v>
@@ -4370,7 +4370,7 @@
         <v>0.0325</v>
       </c>
       <c r="T47" t="n">
-        <v>0</v>
+        <v>0.0308</v>
       </c>
       <c r="U47" t="n">
         <v>0.035</v>
@@ -5438,7 +5438,7 @@
         <v>0.6739000000000001</v>
       </c>
       <c r="L59" t="n">
-        <v>0.6625</v>
+        <v>0.6663</v>
       </c>
       <c r="M59" t="n">
         <v>0.6862999999999999</v>
@@ -6432,13 +6432,13 @@
         <v>0.0401</v>
       </c>
       <c r="I72" t="n">
-        <v>0.02</v>
+        <v>0.0401</v>
       </c>
       <c r="J72" t="n">
-        <v>0.02</v>
+        <v>0.0401</v>
       </c>
       <c r="K72" t="n">
-        <v>0.02</v>
+        <v>0.0401</v>
       </c>
       <c r="L72" t="n">
         <v>0.0401</v>
@@ -7433,16 +7433,16 @@
         <v>0.4396</v>
       </c>
       <c r="I83" t="n">
-        <v>0.4370000000000001</v>
+        <v>0.4376</v>
       </c>
       <c r="J83" t="n">
-        <v>0.4379</v>
+        <v>0.4443</v>
       </c>
       <c r="K83" t="n">
-        <v>0.4349</v>
+        <v>0.4409</v>
       </c>
       <c r="L83" t="n">
-        <v>0.4765</v>
+        <v>0.4816</v>
       </c>
       <c r="M83" t="n">
         <v>0.4654</v>
@@ -7527,25 +7527,25 @@
         <v>0.3413</v>
       </c>
       <c r="J84" t="n">
-        <v>0.3308</v>
+        <v>0.3356</v>
       </c>
       <c r="K84" t="n">
-        <v>0.3254</v>
+        <v>0.3290999999999999</v>
       </c>
       <c r="L84" t="n">
-        <v>0.3442</v>
+        <v>0.3515</v>
       </c>
       <c r="M84" t="n">
-        <v>0.3392</v>
+        <v>0.361</v>
       </c>
       <c r="N84" t="n">
-        <v>0.3449</v>
+        <v>0.3746</v>
       </c>
       <c r="O84" t="n">
-        <v>0.3434</v>
+        <v>0.3892</v>
       </c>
       <c r="P84" t="n">
-        <v>0.358</v>
+        <v>0.3794</v>
       </c>
       <c r="Q84" t="n">
         <v>0.3628</v>
@@ -7630,13 +7630,13 @@
         <v>0.6523</v>
       </c>
       <c r="N85" t="n">
-        <v>0</v>
+        <v>0.6334000000000001</v>
       </c>
       <c r="O85" t="n">
-        <v>0</v>
+        <v>0.6347</v>
       </c>
       <c r="P85" t="n">
-        <v>0</v>
+        <v>0.6053999999999999</v>
       </c>
       <c r="Q85" t="n">
         <v>0.6196</v>
@@ -8257,13 +8257,13 @@
         <v>0</v>
       </c>
       <c r="J94" t="n">
-        <v>0</v>
+        <v>0.0725</v>
       </c>
       <c r="K94" t="n">
-        <v>0</v>
+        <v>0.0755</v>
       </c>
       <c r="L94" t="n">
-        <v>0</v>
+        <v>0.0732</v>
       </c>
       <c r="M94" t="n">
         <v>0</v>
@@ -8360,13 +8360,13 @@
         <v>0.07480000000000001</v>
       </c>
       <c r="N95" t="n">
-        <v>0.02</v>
+        <v>0.0731</v>
       </c>
       <c r="O95" t="n">
-        <v>0.02</v>
+        <v>0.05309999999999999</v>
       </c>
       <c r="P95" t="n">
-        <v>0.02</v>
+        <v>0.0433</v>
       </c>
       <c r="Q95" t="n">
         <v>0.0315</v>
@@ -8451,13 +8451,13 @@
         <v>0.02</v>
       </c>
       <c r="N96" t="n">
-        <v>0.001</v>
+        <v>0.02</v>
       </c>
       <c r="O96" t="n">
-        <v>0.0073</v>
+        <v>0.02</v>
       </c>
       <c r="P96" t="n">
-        <v>0.0011</v>
+        <v>0.02</v>
       </c>
       <c r="Q96" t="n">
         <v>0.02</v>
@@ -8542,13 +8542,13 @@
         <v>0.0012</v>
       </c>
       <c r="N97" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O97" t="n">
-        <v>0</v>
+        <v>0.0073</v>
       </c>
       <c r="P97" t="n">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
       <c r="Q97" t="n">
         <v>0.0008</v>

</xml_diff>